<commit_message>
Update libraries and PCB files
</commit_message>
<xml_diff>
--- a/Connections & PinSchemes/PinsScheme.xlsx
+++ b/Connections & PinSchemes/PinsScheme.xlsx
@@ -113,9 +113,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -124,6 +121,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,7 +408,7 @@
   <dimension ref="B4:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,85 +419,86 @@
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>7</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>6</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>